<commit_message>
Fresh start for Newmarket Streamlit app
</commit_message>
<xml_diff>
--- a/Betting_Simulation/grouped_r_metrics.xlsx
+++ b/Betting_Simulation/grouped_r_metrics.xlsx
@@ -474,19 +474,19 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>67</v>
+        <v>3</v>
       </c>
       <c r="C2" t="n">
-        <v>10.39</v>
+        <v>-3</v>
       </c>
       <c r="D2" t="n">
-        <v>55.38999999999999</v>
+        <v>0</v>
       </c>
       <c r="E2" t="n">
-        <v>-45</v>
+        <v>-3</v>
       </c>
       <c r="F2" t="n">
-        <v>32.8</v>
+        <v>0</v>
       </c>
     </row>
     <row r="3">
@@ -496,19 +496,19 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>32</v>
+        <v>100</v>
       </c>
       <c r="C3" t="n">
-        <v>14</v>
+        <v>56</v>
       </c>
       <c r="D3" t="n">
-        <v>39</v>
+        <v>136</v>
       </c>
       <c r="E3" t="n">
-        <v>-25</v>
+        <v>-80</v>
       </c>
       <c r="F3" t="n">
-        <v>21.9</v>
+        <v>20</v>
       </c>
     </row>
     <row r="4">
@@ -518,20 +518,18 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C4" t="n">
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="D4" t="n">
         <v>0</v>
       </c>
       <c r="E4" t="n">
-        <v>-1</v>
-      </c>
-      <c r="F4" t="n">
-        <v>0</v>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="F4" t="inlineStr"/>
     </row>
     <row r="5">
       <c r="A5" s="1" t="inlineStr">
@@ -651,19 +649,19 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>13</v>
+        <v>6</v>
       </c>
       <c r="C2" t="n">
-        <v>2.63</v>
+        <v>0.5</v>
       </c>
       <c r="D2" t="n">
-        <v>11.63</v>
+        <v>5.5</v>
       </c>
       <c r="E2" t="n">
-        <v>-9</v>
+        <v>-5</v>
       </c>
       <c r="F2" t="n">
-        <v>30.8</v>
+        <v>16.7</v>
       </c>
     </row>
     <row r="3">
@@ -673,19 +671,19 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>38</v>
+        <v>19</v>
       </c>
       <c r="C3" t="n">
-        <v>8.68</v>
+        <v>0</v>
       </c>
       <c r="D3" t="n">
-        <v>33.68</v>
+        <v>17</v>
       </c>
       <c r="E3" t="n">
-        <v>-25</v>
+        <v>-17</v>
       </c>
       <c r="F3" t="n">
-        <v>34.2</v>
+        <v>10.5</v>
       </c>
     </row>
     <row r="4">
@@ -695,19 +693,19 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>49</v>
+        <v>36</v>
       </c>
       <c r="C4" t="n">
-        <v>12.08</v>
+        <v>15</v>
       </c>
       <c r="D4" t="n">
-        <v>49.08</v>
+        <v>44</v>
       </c>
       <c r="E4" t="n">
-        <v>-37</v>
+        <v>-29</v>
       </c>
       <c r="F4" t="n">
-        <v>24.5</v>
+        <v>19.4</v>
       </c>
     </row>
     <row r="5">
@@ -717,18 +715,20 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>0</v>
+        <v>42</v>
       </c>
       <c r="C5" t="n">
-        <v>0</v>
+        <v>37.5</v>
       </c>
       <c r="D5" t="n">
-        <v>0</v>
+        <v>69.5</v>
       </c>
       <c r="E5" t="n">
-        <v>0</v>
-      </c>
-      <c r="F5" t="inlineStr"/>
+        <v>-32</v>
+      </c>
+      <c r="F5" t="n">
+        <v>23.8</v>
+      </c>
     </row>
     <row r="6">
       <c r="A6" s="1" t="inlineStr">
@@ -884,23 +884,23 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>HAMILTON</t>
+          <t>NEWMARKET</t>
         </is>
       </c>
       <c r="B2" t="n">
-        <v>100</v>
+        <v>103</v>
       </c>
       <c r="C2" t="n">
-        <v>23.39</v>
+        <v>53</v>
       </c>
       <c r="D2" t="n">
-        <v>94.39</v>
+        <v>136</v>
       </c>
       <c r="E2" t="n">
-        <v>-71</v>
+        <v>-83</v>
       </c>
       <c r="F2" t="n">
-        <v>29</v>
+        <v>19.4</v>
       </c>
     </row>
   </sheetData>

</xml_diff>